<commit_message>
Changing Temp Code; Before starting TCS v2
</commit_message>
<xml_diff>
--- a/WaterTesting/Tag Results/tags_coefficients.xlsx
+++ b/WaterTesting/Tag Results/tags_coefficients.xlsx
@@ -659,10 +659,10 @@
         <v>22.8482</v>
       </c>
       <c r="G2">
-        <v>22.85223801397142</v>
+        <v>22.852</v>
       </c>
       <c r="I2">
-        <v>0.3477619860285799</v>
+        <v>0.348</v>
       </c>
       <c r="J2">
         <v>0.892</v>
@@ -674,16 +674,16 @@
         <v>22.2039</v>
       </c>
       <c r="N2">
-        <v>22.52604166666667</v>
+        <v>22.526</v>
       </c>
       <c r="O2">
-        <v>22.54669632675027</v>
+        <v>22.547</v>
       </c>
       <c r="P2">
-        <v>0.6739583333333314</v>
+        <v>0.674</v>
       </c>
       <c r="Q2">
-        <v>0.6533036732497273</v>
+        <v>0.653</v>
       </c>
       <c r="R2">
         <v>0.668</v>
@@ -698,13 +698,13 @@
         <v>22.146</v>
       </c>
       <c r="W2">
-        <v>22.19624925781422</v>
+        <v>22.196</v>
       </c>
       <c r="X2">
-        <v>1.053999999999998</v>
+        <v>1.054</v>
       </c>
       <c r="Y2">
-        <v>1.003750742185776</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -721,16 +721,16 @@
         <v>22.5801</v>
       </c>
       <c r="F3">
-        <v>22.6725</v>
+        <v>22.672</v>
       </c>
       <c r="G3">
-        <v>22.72215112349683</v>
+        <v>22.722</v>
       </c>
       <c r="H3">
-        <v>0.5274999999999999</v>
+        <v>0.527</v>
       </c>
       <c r="I3">
-        <v>0.4778488765031739</v>
+        <v>0.478</v>
       </c>
       <c r="J3">
         <v>0.706</v>
@@ -742,16 +742,16 @@
         <v>22.1291</v>
       </c>
       <c r="N3">
-        <v>22.38238095238096</v>
+        <v>22.382</v>
       </c>
       <c r="O3">
-        <v>22.32733082953631</v>
+        <v>22.327</v>
       </c>
       <c r="P3">
-        <v>0.8176190476190435</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="Q3">
-        <v>0.8726691704636913</v>
+        <v>0.873</v>
       </c>
       <c r="R3">
         <v>0.853</v>
@@ -763,16 +763,16 @@
         <v>21.6872</v>
       </c>
       <c r="V3">
-        <v>22.04951219512195</v>
+        <v>22.05</v>
       </c>
       <c r="W3">
-        <v>22.01072549952523</v>
+        <v>22.011</v>
       </c>
       <c r="X3">
-        <v>1.150487804878047</v>
+        <v>1.15</v>
       </c>
       <c r="Y3">
-        <v>1.18927450047477</v>
+        <v>1.189</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -791,17 +791,17 @@
       <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="F4">
-        <v>23.26133333333333</v>
-      </c>
-      <c r="G4">
-        <v>23.28382302313528</v>
-      </c>
-      <c r="H4">
-        <v>0.03866666666666774</v>
-      </c>
-      <c r="I4">
-        <v>0.01617697686472397</v>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
       </c>
       <c r="J4" t="s">
         <v>53</v>
@@ -815,17 +815,17 @@
       <c r="M4" t="s">
         <v>53</v>
       </c>
-      <c r="N4">
-        <v>22.98530303030303</v>
-      </c>
-      <c r="O4">
-        <v>22.99259828607417</v>
-      </c>
-      <c r="P4">
-        <v>0.3146969696969713</v>
-      </c>
-      <c r="Q4">
-        <v>0.3074017139258345</v>
+      <c r="N4" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>53</v>
       </c>
       <c r="R4">
         <v>0.983</v>
@@ -837,10 +837,10 @@
         <v>21.9836</v>
       </c>
       <c r="W4">
-        <v>22.18011627906976</v>
+        <v>22.18</v>
       </c>
       <c r="Y4">
-        <v>1.11988372093024</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -857,16 +857,16 @@
         <v>23.0976</v>
       </c>
       <c r="F5">
-        <v>23.26133333333333</v>
+        <v>23.261</v>
       </c>
       <c r="G5">
-        <v>23.28382302313528</v>
+        <v>23.284</v>
       </c>
       <c r="H5">
-        <v>0.4386666666666663</v>
+        <v>0.039</v>
       </c>
       <c r="I5">
-        <v>0.4161769768647225</v>
+        <v>0.016</v>
       </c>
       <c r="J5">
         <v>0.947</v>
@@ -878,16 +878,16 @@
         <v>22.6604</v>
       </c>
       <c r="N5">
-        <v>22.98530303030303</v>
+        <v>22.985</v>
       </c>
       <c r="O5">
-        <v>22.99259828607417</v>
+        <v>22.993</v>
       </c>
       <c r="P5">
-        <v>0.7146969696969698</v>
+        <v>0.315</v>
       </c>
       <c r="Q5">
-        <v>0.7074017139258331</v>
+        <v>0.307</v>
       </c>
       <c r="R5">
         <v>0.892</v>
@@ -899,16 +899,16 @@
         <v>22.2999</v>
       </c>
       <c r="V5">
-        <v>22.62366666666667</v>
+        <v>22.624</v>
       </c>
       <c r="W5">
-        <v>22.63982095634366</v>
+        <v>22.64</v>
       </c>
       <c r="X5">
-        <v>0.6763333333333357</v>
+        <v>0.676</v>
       </c>
       <c r="Y5">
-        <v>0.6601790436563455</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -924,11 +924,17 @@
       <c r="E6">
         <v>23.0976</v>
       </c>
+      <c r="F6">
+        <v>23.261</v>
+      </c>
       <c r="G6">
-        <v>33.00714285714286</v>
+        <v>23.284</v>
+      </c>
+      <c r="H6">
+        <v>0.439</v>
       </c>
       <c r="I6">
-        <v>0.2928571428571374</v>
+        <v>0.416</v>
       </c>
       <c r="J6">
         <v>0.947</v>
@@ -940,16 +946,16 @@
         <v>22.6604</v>
       </c>
       <c r="N6">
-        <v>32.84</v>
+        <v>22.985</v>
       </c>
       <c r="O6">
-        <v>32.72709395082042</v>
+        <v>22.993</v>
       </c>
       <c r="P6">
-        <v>0.4599999999999937</v>
+        <v>0.715</v>
       </c>
       <c r="Q6">
-        <v>0.5729060491795792</v>
+        <v>0.707</v>
       </c>
       <c r="R6">
         <v>0.892</v>
@@ -961,16 +967,16 @@
         <v>22.2999</v>
       </c>
       <c r="V6">
-        <v>22.62366666666667</v>
+        <v>22.624</v>
       </c>
       <c r="W6">
-        <v>22.63982095634366</v>
+        <v>22.64</v>
       </c>
       <c r="X6">
-        <v>1.076333333333334</v>
+        <v>1.076</v>
       </c>
       <c r="Y6">
-        <v>1.060179043656344</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -986,17 +992,11 @@
       <c r="E7">
         <v>32.9357</v>
       </c>
-      <c r="F7">
-        <v>40.29357142857143</v>
-      </c>
       <c r="G7">
-        <v>40.35561419367172</v>
-      </c>
-      <c r="H7">
-        <v>0.4064285714285703</v>
+        <v>33.007</v>
       </c>
       <c r="I7">
-        <v>0.3443858063282832</v>
+        <v>0.293</v>
       </c>
       <c r="J7">
         <v>0.741</v>
@@ -1008,16 +1008,16 @@
         <v>32.3575</v>
       </c>
       <c r="N7">
-        <v>40.064</v>
+        <v>32.84</v>
       </c>
       <c r="O7">
-        <v>40.08371870105163</v>
+        <v>32.727</v>
       </c>
       <c r="P7">
-        <v>0.6360000000000028</v>
+        <v>0.46</v>
       </c>
       <c r="Q7">
-        <v>0.6162812989483726</v>
+        <v>0.573</v>
       </c>
       <c r="R7">
         <v>0.608</v>
@@ -1029,16 +1029,16 @@
         <v>31.8687</v>
       </c>
       <c r="V7">
-        <v>32.2825</v>
+        <v>32.282</v>
       </c>
       <c r="W7">
-        <v>32.1865610095736</v>
+        <v>32.187</v>
       </c>
       <c r="X7">
-        <v>1.017499999999998</v>
+        <v>1.017</v>
       </c>
       <c r="Y7">
-        <v>1.113438990426395</v>
+        <v>1.113</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1055,16 +1055,16 @@
         <v>40.1468</v>
       </c>
       <c r="F8">
-        <v>50.77999999999999</v>
+        <v>40.294</v>
       </c>
       <c r="G8">
-        <v>50.81265274503978</v>
+        <v>40.356</v>
       </c>
       <c r="H8">
-        <v>-0.279999999999994</v>
+        <v>0.406</v>
       </c>
       <c r="I8">
-        <v>-0.3126527450397845</v>
+        <v>0.344</v>
       </c>
       <c r="J8">
         <v>0.891</v>
@@ -1076,16 +1076,16 @@
         <v>39.8079</v>
       </c>
       <c r="N8">
-        <v>50.67276595744681</v>
+        <v>40.064</v>
       </c>
       <c r="O8">
-        <v>50.68376326986545</v>
+        <v>40.084</v>
       </c>
       <c r="P8">
-        <v>-0.1727659574468063</v>
+        <v>0.636</v>
       </c>
       <c r="Q8">
-        <v>-0.1837632698654517</v>
+        <v>0.616</v>
       </c>
       <c r="R8">
         <v>0.404</v>
@@ -1100,13 +1100,13 @@
         <v>39.86</v>
       </c>
       <c r="W8">
-        <v>40.03771847585158</v>
+        <v>40.038</v>
       </c>
       <c r="X8">
-        <v>0.8400000000000034</v>
+        <v>0.84</v>
       </c>
       <c r="Y8">
-        <v>0.662281524148419</v>
+        <v>0.662</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1123,16 +1123,16 @@
         <v>50.5261</v>
       </c>
       <c r="F9">
-        <v>51.09590909090909</v>
+        <v>50.78</v>
       </c>
       <c r="G9">
-        <v>51.11233411076555</v>
+        <v>50.813</v>
       </c>
       <c r="H9">
-        <v>-0.2959090909090918</v>
+        <v>-0.28</v>
       </c>
       <c r="I9">
-        <v>-0.3123341107655548</v>
+        <v>-0.313</v>
       </c>
       <c r="J9">
         <v>0.944</v>
@@ -1144,16 +1144,16 @@
         <v>50.4144</v>
       </c>
       <c r="N9">
-        <v>50.92633333333332</v>
+        <v>50.673</v>
       </c>
       <c r="O9">
-        <v>50.98832167454265</v>
+        <v>50.684</v>
       </c>
       <c r="P9">
-        <v>-0.1263333333333208</v>
+        <v>-0.173</v>
       </c>
       <c r="Q9">
-        <v>-0.1883216745426495</v>
+        <v>-0.184</v>
       </c>
       <c r="R9">
         <v>0.913</v>
@@ -1165,16 +1165,16 @@
         <v>50.0113</v>
       </c>
       <c r="V9">
-        <v>50.57847826086955</v>
+        <v>50.578</v>
       </c>
       <c r="W9">
-        <v>50.48310009724508</v>
+        <v>50.483</v>
       </c>
       <c r="X9">
-        <v>-0.07847826086954512</v>
+        <v>-0.078</v>
       </c>
       <c r="Y9">
-        <v>0.01689990275492192</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1190,11 +1190,17 @@
       <c r="E10">
         <v>50.8362</v>
       </c>
+      <c r="F10">
+        <v>51.096</v>
+      </c>
       <c r="G10">
-        <v>54.294950310559</v>
+        <v>51.112</v>
+      </c>
+      <c r="H10">
+        <v>-0.296</v>
       </c>
       <c r="I10">
-        <v>-0.2949503105589955</v>
+        <v>-0.312</v>
       </c>
       <c r="J10">
         <v>0.886</v>
@@ -1206,16 +1212,16 @@
         <v>50.7209</v>
       </c>
       <c r="N10">
-        <v>54.17738095238093</v>
+        <v>50.926</v>
       </c>
       <c r="O10">
-        <v>54.20442722426224</v>
+        <v>50.988</v>
       </c>
       <c r="P10">
-        <v>-0.1773809523809291</v>
+        <v>-0.126</v>
       </c>
       <c r="Q10">
-        <v>-0.2044272242622398</v>
+        <v>-0.188</v>
       </c>
       <c r="R10">
         <v>0.966</v>
@@ -1227,16 +1233,16 @@
         <v>50.1229</v>
       </c>
       <c r="V10">
-        <v>50.74431372549019</v>
+        <v>50.744</v>
       </c>
       <c r="W10">
-        <v>50.68905529377616</v>
+        <v>50.689</v>
       </c>
       <c r="X10">
-        <v>0.05568627450980301</v>
+        <v>0.056</v>
       </c>
       <c r="Y10">
-        <v>0.1109447062238402</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1253,10 +1259,10 @@
         <v>53.8933</v>
       </c>
       <c r="G11">
-        <v>53.92012106537529</v>
+        <v>54.295</v>
       </c>
       <c r="I11">
-        <v>0.2798789346247119</v>
+        <v>-0.295</v>
       </c>
       <c r="J11">
         <v>0.857</v>
@@ -1268,16 +1274,16 @@
         <v>53.9229</v>
       </c>
       <c r="N11">
-        <v>54.1796</v>
+        <v>54.177</v>
       </c>
       <c r="O11">
-        <v>54.1895905007902</v>
+        <v>54.204</v>
       </c>
       <c r="P11">
-        <v>0.02040000000000219</v>
+        <v>-0.177</v>
       </c>
       <c r="Q11">
-        <v>0.01040949920980694</v>
+        <v>-0.204</v>
       </c>
       <c r="R11">
         <v>0.702</v>
@@ -1289,16 +1295,16 @@
         <v>53.6483</v>
       </c>
       <c r="V11">
-        <v>54.06428571428572</v>
+        <v>54.064</v>
       </c>
       <c r="W11">
-        <v>53.96970912197885</v>
+        <v>53.97</v>
       </c>
       <c r="X11">
-        <v>-0.06428571428571672</v>
+        <v>-0.064</v>
       </c>
       <c r="Y11">
-        <v>0.03029087802114816</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1315,10 +1321,10 @@
         <v>53.0567</v>
       </c>
       <c r="G12">
-        <v>53.92012106537529</v>
+        <v>53.92</v>
       </c>
       <c r="I12">
-        <v>0.2798789346247119</v>
+        <v>0.28</v>
       </c>
       <c r="J12">
         <v>0.805</v>
@@ -1330,16 +1336,16 @@
         <v>53.8723</v>
       </c>
       <c r="N12">
-        <v>54.15344827586208</v>
+        <v>54.18</v>
       </c>
       <c r="O12">
-        <v>54.12879570783991</v>
+        <v>54.19</v>
       </c>
       <c r="P12">
-        <v>0.04655172413792741</v>
+        <v>0.02</v>
       </c>
       <c r="Q12">
-        <v>0.07120429216009683</v>
+        <v>0.01</v>
       </c>
       <c r="R12">
         <v>0.597</v>
@@ -1354,31 +1360,19 @@
         <v>54.069</v>
       </c>
       <c r="W12">
-        <v>53.98694773107008</v>
+        <v>53.987</v>
       </c>
       <c r="X12">
-        <v>0.1310000000000002</v>
+        <v>0.131</v>
       </c>
       <c r="Y12">
-        <v>0.2130522689299212</v>
+        <v>0.213</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F13">
-        <v>55.64131578947368</v>
-      </c>
-      <c r="G13">
-        <v>55.59459953910527</v>
-      </c>
-      <c r="H13">
-        <v>-0.1413157894736798</v>
-      </c>
-      <c r="I13">
-        <v>-0.09459953910527474</v>
-      </c>
       <c r="J13">
         <v>0.824</v>
       </c>
@@ -1389,16 +1383,16 @@
         <v>53.8498</v>
       </c>
       <c r="N13">
-        <v>55.50692307692308</v>
+        <v>54.153</v>
       </c>
       <c r="O13">
-        <v>55.47383144793635</v>
+        <v>54.129</v>
       </c>
       <c r="P13">
-        <v>-0.006923076923079918</v>
+        <v>0.047</v>
       </c>
       <c r="Q13">
-        <v>0.02616855206365187</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="R13">
         <v>0.545</v>
@@ -1413,13 +1407,13 @@
         <v>54.01</v>
       </c>
       <c r="W13">
-        <v>53.97372420691719</v>
+        <v>53.974</v>
       </c>
       <c r="X13">
-        <v>0.1900000000000048</v>
+        <v>0.19</v>
       </c>
       <c r="Y13">
-        <v>0.226275793082813</v>
+        <v>0.226</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1435,17 +1429,17 @@
       <c r="E14">
         <v>55.3841</v>
       </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" t="s">
-        <v>54</v>
+      <c r="F14">
+        <v>55.641</v>
+      </c>
+      <c r="G14">
+        <v>55.595</v>
+      </c>
+      <c r="H14">
+        <v>-0.141</v>
+      </c>
+      <c r="I14">
+        <v>-0.095</v>
       </c>
       <c r="J14">
         <v>0.885</v>
@@ -1456,17 +1450,17 @@
       <c r="M14">
         <v>55.2027</v>
       </c>
-      <c r="N14" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" t="s">
-        <v>54</v>
-      </c>
-      <c r="P14" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>54</v>
+      <c r="N14">
+        <v>55.507</v>
+      </c>
+      <c r="O14">
+        <v>55.474</v>
+      </c>
+      <c r="P14">
+        <v>-0.007</v>
+      </c>
+      <c r="Q14">
+        <v>0.026</v>
       </c>
       <c r="R14">
         <v>0.747</v>
@@ -1478,16 +1472,16 @@
         <v>54.8739</v>
       </c>
       <c r="V14">
-        <v>55.41500000000001</v>
+        <v>55.415</v>
       </c>
       <c r="W14">
-        <v>55.2969254630922</v>
+        <v>55.297</v>
       </c>
       <c r="X14">
-        <v>0.08499999999999375</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="Y14">
-        <v>0.2030745369077991</v>
+        <v>0.203</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2785,6 +2779,18 @@
       <c r="E4" t="s">
         <v>53</v>
       </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
       <c r="J4" t="s">
         <v>53</v>
       </c>
@@ -2795,6 +2801,18 @@
         <v>53</v>
       </c>
       <c r="M4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3044,30 +3062,6 @@
       </c>
       <c r="E14">
         <v>53.9944</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" t="s">
-        <v>54</v>
-      </c>
-      <c r="N14" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" t="s">
-        <v>54</v>
-      </c>
-      <c r="P14" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>54</v>
       </c>
       <c r="R14">
         <v>1</v>
@@ -4218,10 +4212,10 @@
         <v>22.5291</v>
       </c>
       <c r="G2">
-        <v>22.92621417723621</v>
+        <v>22.926</v>
       </c>
       <c r="I2">
-        <v>0.2737858227637844</v>
+        <v>0.274</v>
       </c>
       <c r="J2">
         <v>0.922</v>
@@ -4233,16 +4227,16 @@
         <v>22.1352</v>
       </c>
       <c r="N2">
-        <v>22.52604166666667</v>
+        <v>22.526</v>
       </c>
       <c r="O2">
-        <v>22.55347479809001</v>
+        <v>22.553</v>
       </c>
       <c r="P2">
-        <v>0.6739583333333314</v>
+        <v>0.674</v>
       </c>
       <c r="Q2">
-        <v>0.6465252019099843</v>
+        <v>0.647</v>
       </c>
       <c r="R2">
         <v>0.752</v>
@@ -4257,13 +4251,13 @@
         <v>22.146</v>
       </c>
       <c r="W2">
-        <v>22.22004583736742</v>
+        <v>22.22</v>
       </c>
       <c r="X2">
-        <v>1.053999999999998</v>
+        <v>1.054</v>
       </c>
       <c r="Y2">
-        <v>0.9799541626325805</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -4280,16 +4274,16 @@
         <v>22.5801</v>
       </c>
       <c r="F3">
-        <v>22.6725</v>
+        <v>22.672</v>
       </c>
       <c r="G3">
-        <v>22.72215112349683</v>
+        <v>22.722</v>
       </c>
       <c r="H3">
-        <v>0.5274999999999999</v>
+        <v>0.527</v>
       </c>
       <c r="I3">
-        <v>0.4778488765031739</v>
+        <v>0.478</v>
       </c>
       <c r="J3">
         <v>0.706</v>
@@ -4301,16 +4295,16 @@
         <v>22.1291</v>
       </c>
       <c r="N3">
-        <v>22.38238095238096</v>
+        <v>22.382</v>
       </c>
       <c r="O3">
-        <v>22.32733082953631</v>
+        <v>22.327</v>
       </c>
       <c r="P3">
-        <v>0.8176190476190435</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="Q3">
-        <v>0.8726691704636913</v>
+        <v>0.873</v>
       </c>
       <c r="R3">
         <v>0.859</v>
@@ -4322,16 +4316,16 @@
         <v>21.6623</v>
       </c>
       <c r="V3">
-        <v>22.04951219512195</v>
+        <v>22.05</v>
       </c>
       <c r="W3">
-        <v>22.01842592598173</v>
+        <v>22.018</v>
       </c>
       <c r="X3">
-        <v>1.150487804878047</v>
+        <v>1.15</v>
       </c>
       <c r="Y3">
-        <v>1.181574074018268</v>
+        <v>1.182</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -4350,17 +4344,17 @@
       <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="F4">
-        <v>23.26133333333333</v>
-      </c>
-      <c r="G4">
-        <v>23.29015757661201</v>
-      </c>
-      <c r="H4">
-        <v>0.03866666666666774</v>
-      </c>
-      <c r="I4">
-        <v>0.009842423387993904</v>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
       </c>
       <c r="J4" t="s">
         <v>53</v>
@@ -4374,17 +4368,17 @@
       <c r="M4" t="s">
         <v>53</v>
       </c>
-      <c r="N4">
-        <v>22.98530303030303</v>
-      </c>
-      <c r="O4">
-        <v>22.99840532230143</v>
-      </c>
-      <c r="P4">
-        <v>0.3146969696969713</v>
-      </c>
-      <c r="Q4">
-        <v>0.3015946776985672</v>
+      <c r="N4" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>53</v>
       </c>
       <c r="R4">
         <v>0.983</v>
@@ -4396,10 +4390,10 @@
         <v>21.9836</v>
       </c>
       <c r="W4">
-        <v>22.18011627906976</v>
+        <v>22.18</v>
       </c>
       <c r="Y4">
-        <v>1.11988372093024</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -4416,16 +4410,16 @@
         <v>23.0515</v>
       </c>
       <c r="F5">
-        <v>23.26133333333333</v>
+        <v>23.261</v>
       </c>
       <c r="G5">
-        <v>23.29015757661201</v>
+        <v>23.29</v>
       </c>
       <c r="H5">
-        <v>0.4386666666666663</v>
+        <v>0.039</v>
       </c>
       <c r="I5">
-        <v>0.4098424233879925</v>
+        <v>0.01</v>
       </c>
       <c r="J5">
         <v>0.947</v>
@@ -4437,16 +4431,16 @@
         <v>22.6348</v>
       </c>
       <c r="N5">
-        <v>22.98530303030303</v>
+        <v>22.985</v>
       </c>
       <c r="O5">
-        <v>22.99840532230143</v>
+        <v>22.998</v>
       </c>
       <c r="P5">
-        <v>0.7146969696969698</v>
+        <v>0.315</v>
       </c>
       <c r="Q5">
-        <v>0.7015946776985658</v>
+        <v>0.302</v>
       </c>
       <c r="R5">
         <v>0.892</v>
@@ -4458,16 +4452,16 @@
         <v>22.2999</v>
       </c>
       <c r="V5">
-        <v>22.62366666666667</v>
+        <v>22.624</v>
       </c>
       <c r="W5">
-        <v>22.63982095634366</v>
+        <v>22.64</v>
       </c>
       <c r="X5">
-        <v>0.6763333333333357</v>
+        <v>0.676</v>
       </c>
       <c r="Y5">
-        <v>0.6601790436563455</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -4483,11 +4477,17 @@
       <c r="E6">
         <v>23.0515</v>
       </c>
+      <c r="F6">
+        <v>23.261</v>
+      </c>
       <c r="G6">
-        <v>33.00714285714286</v>
+        <v>23.29</v>
+      </c>
+      <c r="H6">
+        <v>0.439</v>
       </c>
       <c r="I6">
-        <v>0.2928571428571374</v>
+        <v>0.41</v>
       </c>
       <c r="J6">
         <v>0.947</v>
@@ -4499,16 +4499,16 @@
         <v>22.6348</v>
       </c>
       <c r="N6">
-        <v>32.84</v>
+        <v>22.985</v>
       </c>
       <c r="O6">
-        <v>32.72709395082042</v>
+        <v>22.998</v>
       </c>
       <c r="P6">
-        <v>0.4599999999999937</v>
+        <v>0.715</v>
       </c>
       <c r="Q6">
-        <v>0.5729060491795792</v>
+        <v>0.702</v>
       </c>
       <c r="R6">
         <v>0.892</v>
@@ -4520,16 +4520,16 @@
         <v>22.2999</v>
       </c>
       <c r="V6">
-        <v>22.62366666666667</v>
+        <v>22.624</v>
       </c>
       <c r="W6">
-        <v>22.63982095634366</v>
+        <v>22.64</v>
       </c>
       <c r="X6">
-        <v>1.076333333333334</v>
+        <v>1.076</v>
       </c>
       <c r="Y6">
-        <v>1.060179043656344</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -4545,17 +4545,11 @@
       <c r="E7">
         <v>32.9357</v>
       </c>
-      <c r="F7">
-        <v>40.29357142857143</v>
-      </c>
       <c r="G7">
-        <v>40.36405316120756</v>
-      </c>
-      <c r="H7">
-        <v>0.4064285714285703</v>
+        <v>33.007</v>
       </c>
       <c r="I7">
-        <v>0.3359468387924451</v>
+        <v>0.293</v>
       </c>
       <c r="J7">
         <v>0.741</v>
@@ -4567,16 +4561,16 @@
         <v>32.3575</v>
       </c>
       <c r="N7">
-        <v>40.064</v>
+        <v>32.84</v>
       </c>
       <c r="O7">
-        <v>40.10109802538374</v>
+        <v>32.727</v>
       </c>
       <c r="P7">
-        <v>0.6360000000000028</v>
+        <v>0.46</v>
       </c>
       <c r="Q7">
-        <v>0.5989019746162612</v>
+        <v>0.573</v>
       </c>
       <c r="R7">
         <v>0.748</v>
@@ -4588,16 +4582,16 @@
         <v>31.7906</v>
       </c>
       <c r="V7">
-        <v>32.2825</v>
+        <v>32.282</v>
       </c>
       <c r="W7">
-        <v>32.18914138442593</v>
+        <v>32.189</v>
       </c>
       <c r="X7">
-        <v>1.017499999999998</v>
+        <v>1.017</v>
       </c>
       <c r="Y7">
-        <v>1.110858615574067</v>
+        <v>1.111</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -4614,16 +4608,16 @@
         <v>40.0534</v>
       </c>
       <c r="F8">
-        <v>50.77999999999999</v>
+        <v>40.294</v>
       </c>
       <c r="G8">
-        <v>50.82258744129871</v>
+        <v>40.364</v>
       </c>
       <c r="H8">
-        <v>-0.279999999999994</v>
+        <v>0.406</v>
       </c>
       <c r="I8">
-        <v>-0.3225874412987082</v>
+        <v>0.336</v>
       </c>
       <c r="J8">
         <v>0.82</v>
@@ -4635,16 +4629,16 @@
         <v>39.6964</v>
       </c>
       <c r="N8">
-        <v>50.67276595744681</v>
+        <v>40.064</v>
       </c>
       <c r="O8">
-        <v>50.70143755322055</v>
+        <v>40.101</v>
       </c>
       <c r="P8">
-        <v>-0.1727659574468063</v>
+        <v>0.636</v>
       </c>
       <c r="Q8">
-        <v>-0.2014375532205506</v>
+        <v>0.599</v>
       </c>
       <c r="R8">
         <v>0.635</v>
@@ -4659,13 +4653,13 @@
         <v>39.86</v>
       </c>
       <c r="W8">
-        <v>39.95685302162205</v>
+        <v>39.957</v>
       </c>
       <c r="X8">
-        <v>0.8400000000000034</v>
+        <v>0.84</v>
       </c>
       <c r="Y8">
-        <v>0.7431469783779576</v>
+        <v>0.743</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -4682,16 +4676,16 @@
         <v>50.4668</v>
       </c>
       <c r="F9">
-        <v>51.09590909090909</v>
+        <v>50.78</v>
       </c>
       <c r="G9">
-        <v>51.1384132224247</v>
+        <v>50.823</v>
       </c>
       <c r="H9">
-        <v>-0.2959090909090918</v>
+        <v>-0.28</v>
       </c>
       <c r="I9">
-        <v>-0.3384132224246983</v>
+        <v>-0.323</v>
       </c>
       <c r="J9">
         <v>0.896</v>
@@ -4703,16 +4697,16 @@
         <v>50.3274</v>
       </c>
       <c r="N9">
-        <v>50.92633333333332</v>
+        <v>50.673</v>
       </c>
       <c r="O9">
-        <v>51.00339883876438</v>
+        <v>50.701</v>
       </c>
       <c r="P9">
-        <v>-0.1263333333333208</v>
+        <v>-0.173</v>
       </c>
       <c r="Q9">
-        <v>-0.2033988387643788</v>
+        <v>-0.201</v>
       </c>
       <c r="R9">
         <v>0.9350000000000001</v>
@@ -4724,16 +4718,16 @@
         <v>50.0222</v>
       </c>
       <c r="V9">
-        <v>50.57847826086955</v>
+        <v>50.578</v>
       </c>
       <c r="W9">
-        <v>50.47926209305912</v>
+        <v>50.479</v>
       </c>
       <c r="X9">
-        <v>-0.07847826086954512</v>
+        <v>-0.078</v>
       </c>
       <c r="Y9">
-        <v>0.02073790694088018</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -4749,11 +4743,17 @@
       <c r="E10">
         <v>50.7293</v>
       </c>
+      <c r="F10">
+        <v>51.096</v>
+      </c>
       <c r="G10">
-        <v>53.63226763913389</v>
+        <v>51.138</v>
+      </c>
+      <c r="H10">
+        <v>-0.296</v>
       </c>
       <c r="I10">
-        <v>0.3677323608661069</v>
+        <v>-0.338</v>
       </c>
       <c r="J10">
         <v>0.875</v>
@@ -4765,16 +4765,16 @@
         <v>50.6354</v>
       </c>
       <c r="N10">
-        <v>54.17738095238093</v>
+        <v>50.926</v>
       </c>
       <c r="O10">
-        <v>54.20707140748223</v>
+        <v>51.003</v>
       </c>
       <c r="P10">
-        <v>-0.1773809523809291</v>
+        <v>-0.126</v>
       </c>
       <c r="Q10">
-        <v>-0.207071407482232</v>
+        <v>-0.203</v>
       </c>
       <c r="R10">
         <v>0.979</v>
@@ -4786,16 +4786,16 @@
         <v>50.1029</v>
       </c>
       <c r="V10">
-        <v>50.74431372549019</v>
+        <v>50.744</v>
       </c>
       <c r="W10">
-        <v>50.69500806247252</v>
+        <v>50.695</v>
       </c>
       <c r="X10">
-        <v>0.05568627450980301</v>
+        <v>0.056</v>
       </c>
       <c r="Y10">
-        <v>0.1049919375274797</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -4812,10 +4812,10 @@
         <v>52.3436</v>
       </c>
       <c r="G11">
-        <v>53.83515573283427</v>
+        <v>53.632</v>
       </c>
       <c r="I11">
-        <v>0.3648442671657293</v>
+        <v>0.368</v>
       </c>
       <c r="J11">
         <v>0.905</v>
@@ -4827,16 +4827,16 @@
         <v>53.9081</v>
       </c>
       <c r="N11">
-        <v>54.1796</v>
+        <v>54.177</v>
       </c>
       <c r="O11">
-        <v>54.1895905007902</v>
+        <v>54.207</v>
       </c>
       <c r="P11">
-        <v>0.02040000000000219</v>
+        <v>-0.177</v>
       </c>
       <c r="Q11">
-        <v>0.01040949920980694</v>
+        <v>-0.207</v>
       </c>
       <c r="R11">
         <v>0.762</v>
@@ -4848,16 +4848,16 @@
         <v>53.6472</v>
       </c>
       <c r="V11">
-        <v>54.06428571428572</v>
+        <v>54.064</v>
       </c>
       <c r="W11">
-        <v>53.9698926606767</v>
+        <v>53.97</v>
       </c>
       <c r="X11">
-        <v>-0.06428571428571672</v>
+        <v>-0.064</v>
       </c>
       <c r="Y11">
-        <v>0.03010733932330112</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -4874,10 +4874,10 @@
         <v>52.8792</v>
       </c>
       <c r="G12">
-        <v>52.44021157323681</v>
+        <v>53.835</v>
       </c>
       <c r="I12">
-        <v>1.759788426763194</v>
+        <v>0.365</v>
       </c>
       <c r="J12">
         <v>0.805</v>
@@ -4889,16 +4889,16 @@
         <v>53.8723</v>
       </c>
       <c r="N12">
-        <v>54.15344827586208</v>
+        <v>54.18</v>
       </c>
       <c r="O12">
-        <v>54.12879570783991</v>
+        <v>54.19</v>
       </c>
       <c r="P12">
-        <v>0.04655172413792741</v>
+        <v>0.02</v>
       </c>
       <c r="Q12">
-        <v>0.07120429216009683</v>
+        <v>0.01</v>
       </c>
       <c r="R12">
         <v>0.678</v>
@@ -4913,13 +4913,13 @@
         <v>54.069</v>
       </c>
       <c r="W12">
-        <v>53.98840742396131</v>
+        <v>53.988</v>
       </c>
       <c r="X12">
-        <v>0.1310000000000002</v>
+        <v>0.131</v>
       </c>
       <c r="Y12">
-        <v>0.2115925760386972</v>
+        <v>0.212</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -4935,17 +4935,11 @@
       <c r="E13">
         <v>50.2358</v>
       </c>
-      <c r="F13">
-        <v>55.64131578947368</v>
-      </c>
       <c r="G13">
-        <v>55.59829855949237</v>
-      </c>
-      <c r="H13">
-        <v>-0.1413157894736798</v>
+        <v>52.44</v>
       </c>
       <c r="I13">
-        <v>-0.09829855949237043</v>
+        <v>1.76</v>
       </c>
       <c r="J13">
         <v>0.824</v>
@@ -4957,16 +4951,16 @@
         <v>53.8498</v>
       </c>
       <c r="N13">
-        <v>55.50692307692308</v>
+        <v>54.153</v>
       </c>
       <c r="O13">
-        <v>55.47383144793635</v>
+        <v>54.129</v>
       </c>
       <c r="P13">
-        <v>-0.006923076923079918</v>
+        <v>0.047</v>
       </c>
       <c r="Q13">
-        <v>0.02616855206365187</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="R13">
         <v>0.656</v>
@@ -4981,13 +4975,13 @@
         <v>54.01</v>
       </c>
       <c r="W13">
-        <v>53.97659932073429</v>
+        <v>53.977</v>
       </c>
       <c r="X13">
-        <v>0.1900000000000048</v>
+        <v>0.19</v>
       </c>
       <c r="Y13">
-        <v>0.2234006792657084</v>
+        <v>0.223</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -5003,17 +4997,17 @@
       <c r="E14">
         <v>55.3629</v>
       </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" t="s">
-        <v>54</v>
+      <c r="F14">
+        <v>55.641</v>
+      </c>
+      <c r="G14">
+        <v>55.598</v>
+      </c>
+      <c r="H14">
+        <v>-0.141</v>
+      </c>
+      <c r="I14">
+        <v>-0.098</v>
       </c>
       <c r="J14">
         <v>0.885</v>
@@ -5024,17 +5018,17 @@
       <c r="M14">
         <v>55.2027</v>
       </c>
-      <c r="N14" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" t="s">
-        <v>54</v>
-      </c>
-      <c r="P14" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>54</v>
+      <c r="N14">
+        <v>55.507</v>
+      </c>
+      <c r="O14">
+        <v>55.474</v>
+      </c>
+      <c r="P14">
+        <v>-0.007</v>
+      </c>
+      <c r="Q14">
+        <v>0.026</v>
       </c>
       <c r="R14">
         <v>0.791</v>
@@ -5046,16 +5040,16 @@
         <v>54.8781</v>
       </c>
       <c r="V14">
-        <v>55.41500000000001</v>
+        <v>55.415</v>
       </c>
       <c r="W14">
-        <v>55.29534034815359</v>
+        <v>55.295</v>
       </c>
       <c r="X14">
-        <v>0.08499999999999375</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="Y14">
-        <v>0.2046596518464057</v>
+        <v>0.205</v>
       </c>
     </row>
     <row r="15" spans="1:25">

</xml_diff>